<commit_message>
Just for recording. KVS definition sheet is defined.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoKeyGeneratorKtTask.xlsx
+++ b/meta/program/BlancoKeyGeneratorKtTask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoKeyGeneratorKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0821FED4-5965-3945-96A6-0D83804D9DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2CC349-E0D0-BB40-BB9D-86598E4A1DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,8 +378,7 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>キー定義書からソースコードを自動生成する BlancoKeyGeneratorKtのAntTaskです。</t>
-    <phoneticPr fontId="5"/>
+    <t>キーバリューストアテーブル定義書からソースコードを自動生成する BlancoKeyGeneratorKtのAntTaskです。</t>
   </si>
 </sst>
 </file>
@@ -986,6 +985,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1016,28 +1037,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1457,10 +1456,10 @@
       <c r="F5"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="84" t="s">
+      <c r="A6" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="84"/>
+      <c r="B6" s="72"/>
       <c r="C6" s="6" t="s">
         <v>52</v>
       </c>
@@ -1470,10 +1469,10 @@
       <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="84"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="6" t="s">
         <v>53</v>
       </c>
@@ -1484,10 +1483,10 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="84" t="s">
+      <c r="A8" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="84"/>
+      <c r="B8" s="72"/>
       <c r="C8" s="6" t="s">
         <v>54</v>
       </c>
@@ -1498,10 +1497,10 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="84"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="11" t="s">
         <v>7</v>
       </c>
@@ -1533,38 +1532,38 @@
       <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="13.5" customHeight="1">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="89" t="s">
+      <c r="C12" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="90" t="s">
+      <c r="D12" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="91" t="s">
+      <c r="E12" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="82" t="s">
+      <c r="F12" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="83"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="83"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="91"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="88"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="91"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="83"/>
+      <c r="A13" s="76"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
     </row>
     <row r="14" spans="1:9" ht="27" customHeight="1">
       <c r="A14" s="44">
@@ -1580,12 +1579,12 @@
         <v>13</v>
       </c>
       <c r="E14" s="48"/>
-      <c r="F14" s="85" t="s">
+      <c r="F14" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="87"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="75"/>
     </row>
     <row r="15" spans="1:9" ht="27" customHeight="1">
       <c r="A15" s="49">
@@ -1601,12 +1600,12 @@
       <c r="E15" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="78" t="s">
+      <c r="F15" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="79"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="80"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="88"/>
     </row>
     <row r="16" spans="1:9" ht="27" customHeight="1">
       <c r="A16" s="49">
@@ -1622,12 +1621,12 @@
       <c r="E16" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="81" t="s">
+      <c r="F16" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="79"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="80"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="88"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="49">
@@ -1704,12 +1703,12 @@
       <c r="E20" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="75" t="s">
+      <c r="F20" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="76"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="77"/>
+      <c r="G20" s="84"/>
+      <c r="H20" s="84"/>
+      <c r="I20" s="85"/>
     </row>
     <row r="21" spans="1:10" ht="52" customHeight="1">
       <c r="A21" s="49">
@@ -1726,12 +1725,12 @@
       <c r="E21" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="72" t="s">
+      <c r="F21" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="73"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="74"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="81"/>
+      <c r="I21" s="82"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="49">
@@ -1851,6 +1850,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F12:I13"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -1861,11 +1865,6 @@
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F12:I13"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="4">

</xml_diff>